<commit_message>
Data Cleansing - part 1 completed
</commit_message>
<xml_diff>
--- a/Data_Dictionary.xlsx
+++ b/Data_Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehaljadhav/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehaljadhav/Documents/Project/IIITB/Loan_CaseStudy_EDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EABFD85-8945-C146-AB30-FEF3C1F470E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A235606C-D76C-2C46-9A27-B30FC0C6644B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1813,9 +1813,9 @@
   </sheetPr>
   <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2152,7 +2152,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2783,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>

</xml_diff>